<commit_message>
changed to custom tubes file path
</commit_message>
<xml_diff>
--- a/src-tauri/Tubes.xlsx
+++ b/src-tauri/Tubes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve"> C</t>
   </si>
@@ -22,34 +22,7 @@
     <t xml:space="preserve"> 1</t>
   </si>
   <si>
-    <t>5/10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10</t>
+    <t>1/19</t>
   </si>
 </sst>
 </file>
@@ -385,7 +358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,132 +378,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>